<commit_message>
Implemented comments for all classes.
</commit_message>
<xml_diff>
--- a/SAF/src/test/resources/testdata.xlsx
+++ b/SAF/src/test/resources/testdata.xlsx
@@ -440,7 +440,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -543,7 +543,7 @@
         <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Fixed spelling mistake in DynamicXpath Class. Added the code to implement multiple iteration based on test data sheet.Fixed an copy paste error in Logstatus.java
</commit_message>
<xml_diff>
--- a/SAF/src/test/resources/testdata.xlsx
+++ b/SAF/src/test/resources/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RunManager" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -84,6 +84,42 @@
   </si>
   <si>
     <t>Test Case 3</t>
+  </si>
+  <si>
+    <t>valueforsearch</t>
+  </si>
+  <si>
+    <t>automation</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t>efgh</t>
+  </si>
+  <si>
+    <t>4567</t>
+  </si>
+  <si>
+    <t>jbvb</t>
+  </si>
+  <si>
+    <t>987</t>
+  </si>
+  <si>
+    <t>selenium</t>
+  </si>
+  <si>
+    <t>hgb1</t>
+  </si>
+  <si>
+    <t>jnh</t>
+  </si>
+  <si>
+    <t>appium</t>
+  </si>
+  <si>
+    <t>test11</t>
   </si>
 </sst>
 </file>
@@ -439,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -559,10 +595,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -570,7 +606,7 @@
     <col min="1" max="1" width="38.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -580,8 +616,11 @@
       <c r="C1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -591,8 +630,11 @@
       <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -601,12 +643,72 @@
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="Dhl@1234"/>
     <hyperlink ref="C3" r:id="rId2" display="Dhl@1234"/>
+    <hyperlink ref="C4" r:id="rId3" display="Dhl@1234"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Optimised with Base Page, Base Test and Now it supports parallel execution
</commit_message>
<xml_diff>
--- a/SAF/src/test/resources/testdata.xlsx
+++ b/SAF/src/test/resources/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="RunManager" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -96,9 +96,6 @@
   </si>
   <si>
     <t>efgh</t>
-  </si>
-  <si>
-    <t>4567</t>
   </si>
   <si>
     <t>jbvb</t>
@@ -475,18 +472,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.90625" customWidth="1"/>
-    <col min="2" max="2" width="50.36328125" customWidth="1"/>
-    <col min="4" max="4" width="20.453125" customWidth="1"/>
+    <col min="1" max="1" width="43.85546875" customWidth="1"/>
+    <col min="2" max="2" width="50.42578125" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -503,7 +500,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -520,7 +517,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -537,7 +534,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -554,7 +551,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -562,7 +559,7 @@
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>14</v>
@@ -571,7 +568,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -597,16 +594,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.6328125" customWidth="1"/>
+    <col min="1" max="1" width="39.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -620,7 +618,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -634,7 +632,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -648,67 +646,60 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C4" s="1"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
       <c r="B5" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="C5" s="2"/>
       <c r="D5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
       <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" t="s">
         <v>29</v>
       </c>
-      <c r="D6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
       <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" t="s">
         <v>32</v>
-      </c>
-      <c r="D7" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="Dhl@1234"/>
     <hyperlink ref="C3" r:id="rId2" display="Dhl@1234"/>
-    <hyperlink ref="C4" r:id="rId3" display="Dhl@1234"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Made the Extent Report Thread Safe
</commit_message>
<xml_diff>
--- a/SAF/src/test/resources/testdata.xlsx
+++ b/SAF/src/test/resources/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RunManager" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="34">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -472,7 +472,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -594,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,7 +654,9 @@
         <v>11</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">

</xml_diff>

<commit_message>
Included WebDriverManager, Optimised Page Classes
</commit_message>
<xml_diff>
--- a/SAF/src/test/resources/testdata.xlsx
+++ b/SAF/src/test/resources/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="RunManager" sheetId="1" r:id="rId1"/>
@@ -472,18 +472,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="43.85546875" customWidth="1"/>
-    <col min="2" max="2" width="50.42578125" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="43.81640625" customWidth="1"/>
+    <col min="2" max="2" width="50.453125" customWidth="1"/>
+    <col min="4" max="4" width="20.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -500,7 +500,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -517,7 +517,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -534,7 +534,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -551,7 +551,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -594,17 +594,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39.5703125" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="39.54296875" customWidth="1"/>
+    <col min="4" max="4" width="13.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -618,7 +618,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -632,7 +632,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -646,7 +646,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -658,7 +658,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -670,7 +670,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -684,7 +684,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
Implemented support for Docker,Zalenium and more optimization of codes
</commit_message>
<xml_diff>
--- a/SAF/src/test/resources/testdata.xlsx
+++ b/SAF/src/test/resources/testdata.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -26,18 +26,12 @@
     <t>checkWhetherGlobalViewIsSelectedByDefault</t>
   </si>
   <si>
-    <t>Validate whether the default view selected is Global View</t>
-  </si>
-  <si>
     <t>Test Case Description</t>
   </si>
   <si>
     <t>validateEnteringShipmentID</t>
   </si>
   <si>
-    <t>Validate whether the user can able to enter shipmentID</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -60,9 +54,6 @@
   </si>
   <si>
     <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
   </si>
   <si>
     <t>Priority</t>
@@ -470,16 +461,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="43.81640625" customWidth="1"/>
-    <col min="2" max="2" width="50.453125" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" customWidth="1"/>
+    <col min="2" max="2" width="28.6328125" customWidth="1"/>
     <col min="4" max="4" width="20.453125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -488,101 +479,67 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
         <v>13</v>
-      </c>
-      <c r="E1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -609,13 +566,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -623,79 +580,79 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added code to open results after execution. Removed SeleniumUtils Added reusable methods to Base Page
</commit_message>
<xml_diff>
--- a/SAF/src/test/resources/testdata.xlsx
+++ b/SAF/src/test/resources/testdata.xlsx
@@ -464,7 +464,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -552,7 +552,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
First tests for sauceDemo page
</commit_message>
<xml_diff>
--- a/SAF/src/test/resources/testdata.xlsx
+++ b/SAF/src/test/resources/testdata.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10708"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61FA4806-487D-4A46-B414-4496CDEF6A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="32180" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RunManager" sheetId="1" r:id="rId1"/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="39">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -32,88 +33,112 @@
     <t>validateEnteringShipmentID</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>InvocationCount</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>Test case 1</t>
+  </si>
+  <si>
+    <t>Test Case 2</t>
+  </si>
+  <si>
+    <t>test3</t>
+  </si>
+  <si>
+    <t>Test Case 3</t>
+  </si>
+  <si>
+    <t>valueforsearch</t>
+  </si>
+  <si>
+    <t>automation</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t>efgh</t>
+  </si>
+  <si>
+    <t>jbvb</t>
+  </si>
+  <si>
+    <t>987</t>
+  </si>
+  <si>
+    <t>selenium</t>
+  </si>
+  <si>
+    <t>appium</t>
+  </si>
+  <si>
+    <t>test11</t>
+  </si>
+  <si>
     <t>No</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>abcd</t>
-  </si>
-  <si>
-    <t>1234</t>
-  </si>
-  <si>
-    <t>InvocationCount</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Priority</t>
-  </si>
-  <si>
-    <t>test1</t>
-  </si>
-  <si>
-    <t>test2</t>
-  </si>
-  <si>
-    <t>Test case 1</t>
-  </si>
-  <si>
-    <t>Test Case 2</t>
-  </si>
-  <si>
-    <t>test3</t>
-  </si>
-  <si>
-    <t>Test Case 3</t>
-  </si>
-  <si>
-    <t>valueforsearch</t>
-  </si>
-  <si>
-    <t>automation</t>
-  </si>
-  <si>
-    <t>testing</t>
-  </si>
-  <si>
-    <t>efgh</t>
-  </si>
-  <si>
-    <t>jbvb</t>
-  </si>
-  <si>
-    <t>987</t>
-  </si>
-  <si>
-    <t>selenium</t>
-  </si>
-  <si>
-    <t>hgb1</t>
-  </si>
-  <si>
-    <t>jnh</t>
-  </si>
-  <si>
-    <t>appium</t>
-  </si>
-  <si>
-    <t>test11</t>
+    <t>standard_user</t>
+  </si>
+  <si>
+    <t>secret_sauce</t>
+  </si>
+  <si>
+    <t>login_validUsername_invalidPassword</t>
+  </si>
+  <si>
+    <t>aaa</t>
+  </si>
+  <si>
+    <t>pwdpwd</t>
+  </si>
+  <si>
+    <t>login_validUsername_validPassword</t>
+  </si>
+  <si>
+    <t>login_invalidUsername_validPassword</t>
+  </si>
+  <si>
+    <t>useruser</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -250,6 +275,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -285,6 +327,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -460,21 +519,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" customWidth="1"/>
-    <col min="2" max="2" width="28.6328125" customWidth="1"/>
-    <col min="4" max="4" width="20.453125" customWidth="1"/>
+    <col min="1" max="1" width="32.6640625" customWidth="1"/>
+    <col min="2" max="2" width="37.5" customWidth="1"/>
+    <col min="4" max="4" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -485,61 +544,112 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
       <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>12</v>
+      <c r="D5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -548,117 +658,147 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="39.54296875" customWidth="1"/>
-    <col min="4" max="4" width="13.81640625" customWidth="1"/>
+    <col min="1" max="1" width="39.5" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
       <c r="D1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="D2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="D3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" t="s">
-        <v>29</v>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="Dhl@1234"/>
-    <hyperlink ref="C3" r:id="rId2" display="Dhl@1234"/>
+    <hyperlink ref="C2" r:id="rId1" display="Dhl@1234" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" display="Dhl@1234" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>